<commit_message>
updated test output based on changes to readme
</commit_message>
<xml_diff>
--- a/test_data/bsDataDictionary_Psets-out.xlsx
+++ b/test_data/bsDataDictionary_Psets-out.xlsx
@@ -15,44 +15,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>xlsx_params</t>
+  </si>
+  <si>
+    <t>xlsx_exporter</t>
+  </si>
+  <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>IfcProductDataTemplate</t>
+  </si>
+  <si>
+    <t>&lt;class 'templaterdefs.XlsxTable'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;function df_to_sheet_table at 0x7f55e635f700&gt;</t>
+  </si>
+  <si>
+    <t>J4321</t>
+  </si>
+  <si>
+    <t>20210414</t>
+  </si>
+  <si>
+    <t>gunstonej</t>
+  </si>
   <si>
     <t>index</t>
   </si>
   <si>
-    <t>IfcProductDataTemplate</t>
-  </si>
-  <si>
-    <t>xlsx_params</t>
-  </si>
-  <si>
-    <t>xlsx_exporter</t>
-  </si>
-  <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>&lt;class 'templaterdefs.XlsxTable'&gt;</t>
-  </si>
-  <si>
-    <t>&lt;function df_to_sheet_table at 0x7fb9bdfec700&gt;</t>
-  </si>
-  <si>
-    <t>J4321</t>
-  </si>
-  <si>
-    <t>20210414</t>
-  </si>
-  <si>
-    <t>gunstonej</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -63,9 +66,6 @@
   </si>
   <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>sheet_name</t>
   </si>
   <si>
     <t>description</t>
@@ -232,11 +232,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="IfcProductDataTemplate"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" totalsRowShown="0">
+  <autoFilter ref="A1:F2"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="sheet_name"/>
+    <tableColumn id="2" name="xlsx_params"/>
+    <tableColumn id="3" name="xlsx_exporter"/>
+    <tableColumn id="4" name="JobNo"/>
+    <tableColumn id="5" name="Date"/>
+    <tableColumn id="6" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -541,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -553,54 +557,46 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" style="1" customWidth="1"/>
+    <col min="2" max="7" width="40.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -637,24 +633,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
@@ -688,7 +684,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>20</v>
@@ -705,7 +701,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -722,7 +718,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>

</xml_diff>